<commit_message>
add arr dep const, and bug fixes
</commit_message>
<xml_diff>
--- a/center-scheduling/data/01_raw/center_data.xlsx
+++ b/center-scheduling/data/01_raw/center_data.xlsx
@@ -6,7 +6,11 @@
     <sheet name="center_hours" sheetId="1" r:id="rId1"/>
     <sheet name="staff_child" sheetId="2" r:id="rId2"/>
     <sheet name="absences" sheetId="3" r:id="rId3"/>
-    <sheet name="example_out" sheetId="4" r:id="rId4"/>
+    <sheet name="roles" sheetId="4" r:id="rId4"/>
+    <sheet name="ref outputs-&gt;" sheetId="5" r:id="rId5"/>
+    <sheet name="missing " sheetId="6" r:id="rId6"/>
+    <sheet name="example_out" sheetId="7" r:id="rId7"/>
+    <sheet name="Monday Example" sheetId="8" r:id="rId8"/>
   </sheets>
 </workbook>
 </file>
@@ -480,7 +484,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -490,143 +494,385 @@
         <v>Child</v>
       </c>
       <c r="B1" t="str">
-        <v>Staff</v>
+        <v xml:space="preserve">Mario </v>
       </c>
       <c r="C1" t="str">
-        <v>Role</v>
+        <v xml:space="preserve">Luigi </v>
+      </c>
+      <c r="D1" t="str">
+        <v xml:space="preserve">Peach </v>
+      </c>
+      <c r="E1" t="str">
+        <v xml:space="preserve">Daisy </v>
+      </c>
+      <c r="F1" t="str">
+        <v xml:space="preserve">Toad </v>
+      </c>
+      <c r="G1" t="str">
+        <v xml:space="preserve">Bowser </v>
+      </c>
+      <c r="H1" t="str">
+        <v>Frodo</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Sam</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Legolas</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Gimli</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Aragorn</v>
+      </c>
+      <c r="M1" t="str">
+        <v xml:space="preserve">Gandalf </v>
+      </c>
+      <c r="N1" t="str">
+        <v>Thor</v>
+      </c>
+      <c r="O1" t="str">
+        <v>Iron Man</v>
+      </c>
+      <c r="P1" t="str">
+        <v xml:space="preserve">Black Widow </v>
+      </c>
+      <c r="Q1" t="str">
+        <v xml:space="preserve">Hulk </v>
+      </c>
+      <c r="R1" t="str">
+        <v>Spiderman</v>
+      </c>
+      <c r="S1" t="str">
+        <v xml:space="preserve">Arrow </v>
+      </c>
+      <c r="T1" t="str">
+        <v xml:space="preserve">Batman </v>
+      </c>
+      <c r="U1" t="str">
+        <v>Superman</v>
+      </c>
+      <c r="V1" t="str">
+        <v xml:space="preserve">Flash </v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>AA</v>
+        <v xml:space="preserve">lime green </v>
       </c>
       <c r="B2" t="str">
-        <v>Sunya</v>
+        <v>x</v>
       </c>
       <c r="C2" t="str">
-        <v>SBA</v>
+        <v>x</v>
+      </c>
+      <c r="D2" t="str">
+        <v>x</v>
+      </c>
+      <c r="U2" t="str">
+        <v>x</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>AA</v>
+        <v xml:space="preserve">pale yellow </v>
       </c>
       <c r="B3" t="str">
-        <v>Link</v>
+        <v>x</v>
       </c>
       <c r="C3" t="str">
-        <v>Tech</v>
+        <v>x</v>
+      </c>
+      <c r="F3" t="str">
+        <v>x</v>
+      </c>
+      <c r="G3" t="str">
+        <v>x</v>
+      </c>
+      <c r="L3" t="str">
+        <v>x</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>BB</v>
+        <v xml:space="preserve">dark blue </v>
       </c>
       <c r="B4" t="str">
-        <v>Link</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Tech</v>
+        <v>x</v>
+      </c>
+      <c r="F4" t="str">
+        <v>x</v>
+      </c>
+      <c r="G4" t="str">
+        <v>x</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>BB</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Sunya</v>
+        <v>light purple</v>
       </c>
       <c r="C5" t="str">
-        <v>SBA</v>
+        <v>x</v>
+      </c>
+      <c r="D5" t="str">
+        <v>x</v>
+      </c>
+      <c r="E5" t="str">
+        <v>x</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>CC</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Sunya</v>
-      </c>
-      <c r="C6" t="str">
-        <v>SBA</v>
+        <v>light orange</v>
+      </c>
+      <c r="D6" t="str">
+        <v>x</v>
+      </c>
+      <c r="F6" t="str">
+        <v>x</v>
+      </c>
+      <c r="O6" t="str">
+        <v>x</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>CC</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Mario</v>
-      </c>
-      <c r="C7" t="str">
-        <v>Tech</v>
+        <v>red</v>
+      </c>
+      <c r="E7" t="str">
+        <v>x</v>
+      </c>
+      <c r="F7" t="str">
+        <v>x</v>
+      </c>
+      <c r="G7" t="str">
+        <v>x</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>BB</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Zelda</v>
+        <v xml:space="preserve">dark green </v>
       </c>
       <c r="C8" t="str">
-        <v>Tech</v>
+        <v>x</v>
+      </c>
+      <c r="H8" t="str">
+        <v>x</v>
+      </c>
+      <c r="I8" t="str">
+        <v>x</v>
+      </c>
+      <c r="J8" t="str">
+        <v>x</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>AA</v>
-      </c>
-      <c r="B9" t="str">
-        <v>Ganon</v>
-      </c>
-      <c r="C9" t="str">
-        <v>BS</v>
+        <v xml:space="preserve">pink </v>
+      </c>
+      <c r="F9" t="str">
+        <v>x</v>
+      </c>
+      <c r="H9" t="str">
+        <v>x</v>
+      </c>
+      <c r="I9" t="str">
+        <v>x</v>
+      </c>
+      <c r="J9" t="str">
+        <v>x</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>BB</v>
-      </c>
-      <c r="B10" t="str">
-        <v>Ganon</v>
-      </c>
-      <c r="C10" t="str">
-        <v>BS</v>
+        <v>light blue</v>
+      </c>
+      <c r="H10" t="str">
+        <v>x</v>
+      </c>
+      <c r="L10" t="str">
+        <v>x</v>
+      </c>
+      <c r="M10" t="str">
+        <v>x</v>
+      </c>
+      <c r="O10" t="str">
+        <v>x</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>CC</v>
-      </c>
-      <c r="B11" t="str">
-        <v>Ganon</v>
-      </c>
-      <c r="C11" t="str">
-        <v>BS</v>
+        <v xml:space="preserve">grey </v>
+      </c>
+      <c r="H11" t="str">
+        <v>x</v>
+      </c>
+      <c r="L11" t="str">
+        <v>x</v>
+      </c>
+      <c r="M11" t="str">
+        <v>x</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>AA</v>
-      </c>
-      <c r="B12" t="str">
-        <v>Zelda</v>
-      </c>
-      <c r="C12" t="str">
-        <v>Tech</v>
+        <v xml:space="preserve">light grey </v>
+      </c>
+      <c r="L12" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>sky blue</v>
+      </c>
+      <c r="O13" t="str">
+        <v>x</v>
+      </c>
+      <c r="P13" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>yellow</v>
+      </c>
+      <c r="M14" t="str">
+        <v>2.5</v>
+      </c>
+      <c r="P14" t="str">
+        <v>x</v>
+      </c>
+      <c r="Q14" t="str">
+        <v>x</v>
+      </c>
+      <c r="R14" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v xml:space="preserve">teal </v>
+      </c>
+      <c r="N15" t="str">
+        <v>x</v>
+      </c>
+      <c r="R15" t="str">
+        <v>x</v>
+      </c>
+      <c r="T15" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>purple</v>
+      </c>
+      <c r="N16" t="str">
+        <v>x</v>
+      </c>
+      <c r="O16" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>dark purple</v>
+      </c>
+      <c r="O17" t="str">
+        <v>x</v>
+      </c>
+      <c r="P17" t="str">
+        <v>x</v>
+      </c>
+      <c r="Q17" t="str">
+        <v>x</v>
+      </c>
+      <c r="R17" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v xml:space="preserve">dark pink </v>
+      </c>
+      <c r="Q18" t="str">
+        <v>x</v>
+      </c>
+      <c r="R18" t="str">
+        <v>x</v>
+      </c>
+      <c r="T18" t="str">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v xml:space="preserve">tan </v>
+      </c>
+      <c r="C19" t="str">
+        <v>x</v>
+      </c>
+      <c r="T19" t="str">
+        <v>x</v>
+      </c>
+      <c r="V19" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v xml:space="preserve">dark orange </v>
+      </c>
+      <c r="B20" t="str">
+        <v>x</v>
+      </c>
+      <c r="I20" t="str">
+        <v>2.5</v>
+      </c>
+      <c r="U20" t="str">
+        <v>x</v>
+      </c>
+      <c r="V20" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>maroon</v>
+      </c>
+      <c r="R21" t="str">
+        <v>x</v>
+      </c>
+      <c r="U21" t="str">
+        <v>x</v>
+      </c>
+      <c r="V21" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>dark dark blue</v>
+      </c>
+      <c r="T22" t="str">
+        <v>x</v>
+      </c>
+      <c r="V22" t="str">
+        <v>x</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:V22"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -647,88 +893,708 @@
       <c r="E1" t="str">
         <v>Type</v>
       </c>
+      <c r="F1" t="str">
+        <v>Occurrence</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Sunya</v>
+        <v xml:space="preserve">dark pink </v>
       </c>
       <c r="B2" t="str">
-        <v>Tue</v>
+        <v>Mon</v>
+      </c>
+      <c r="D2" t="str">
+        <v>10:00</v>
       </c>
       <c r="E2" t="str">
-        <v>PTO</v>
+        <v xml:space="preserve">late arrival </v>
+      </c>
+      <c r="F2" t="str">
+        <v xml:space="preserve">weekly </v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Sunya</v>
+        <v xml:space="preserve">light blue </v>
       </c>
       <c r="B3" t="str">
-        <v>Wed</v>
+        <v>Mon</v>
       </c>
       <c r="C3" t="str">
-        <v>12</v>
+        <v>9:30</v>
       </c>
       <c r="D3" t="str">
-        <v>13</v>
+        <v>10:00</v>
       </c>
       <c r="E3" t="str">
-        <v>Parent training</v>
+        <v xml:space="preserve">speech </v>
+      </c>
+      <c r="F3" t="str">
+        <v xml:space="preserve">weekly </v>
       </c>
     </row>
     <row r="4">
+      <c r="A4" t="str">
+        <v xml:space="preserve">dark blue </v>
+      </c>
       <c r="B4" t="str">
-        <v>Thu</v>
+        <v>Mon</v>
       </c>
       <c r="C4" t="str">
         <v>16</v>
       </c>
       <c r="D4" t="str">
-        <v>16.50</v>
+        <v>11:30</v>
       </c>
       <c r="E4" t="str">
-        <v>Team meeting</v>
+        <v xml:space="preserve">late arrival </v>
+      </c>
+      <c r="F4" t="str">
+        <v xml:space="preserve">weekly </v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>CC</v>
+        <v xml:space="preserve">dark dark blue </v>
+      </c>
+      <c r="B5" t="str">
+        <v xml:space="preserve">Mon </v>
       </c>
       <c r="C5" t="str">
-        <v>12</v>
+        <v>12:30</v>
       </c>
       <c r="D5" t="str">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E5" t="str">
-        <v>Nap</v>
+        <v xml:space="preserve">leaves early </v>
+      </c>
+      <c r="F5" t="str">
+        <v xml:space="preserve">weekly </v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>CC</v>
+        <v xml:space="preserve">dark dark blue </v>
       </c>
       <c r="B6" t="str">
         <v>Wed</v>
       </c>
       <c r="C6" t="str">
-        <v>15</v>
-      </c>
-      <c r="D6" t="str">
-        <v>16</v>
+        <v>12:30</v>
       </c>
       <c r="E6" t="str">
-        <v>Speech</v>
+        <v xml:space="preserve">leaves early </v>
+      </c>
+      <c r="F6" t="str">
+        <v xml:space="preserve">weekly </v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v xml:space="preserve">red </v>
+      </c>
+      <c r="D7" t="str">
+        <v>9:30</v>
+      </c>
+      <c r="E7" t="str">
+        <v xml:space="preserve">late arrival </v>
+      </c>
+      <c r="F7" t="str">
+        <v xml:space="preserve">weekly </v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v xml:space="preserve">red </v>
+      </c>
+      <c r="C8" t="str">
+        <v>1:00</v>
+      </c>
+      <c r="E8" t="str">
+        <v xml:space="preserve">leaves early </v>
+      </c>
+      <c r="F8" t="str">
+        <v xml:space="preserve">weekly </v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v xml:space="preserve">dark green </v>
+      </c>
+      <c r="B9" t="str">
+        <v>Mon</v>
+      </c>
+      <c r="C9" t="str">
+        <v>2:45</v>
+      </c>
+      <c r="E9" t="str">
+        <v xml:space="preserve">leaves early </v>
+      </c>
+      <c r="F9" t="str">
+        <v>once</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>light purple</v>
+      </c>
+      <c r="C10" t="str">
+        <v>1:30</v>
+      </c>
+      <c r="D10" t="str">
+        <v>2:30</v>
+      </c>
+      <c r="E10" t="str">
+        <v xml:space="preserve">nap </v>
+      </c>
+      <c r="F10" t="str">
+        <v xml:space="preserve">weekly </v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v xml:space="preserve">dark dark blue </v>
+      </c>
+      <c r="B11" t="str">
+        <v>Tue</v>
+      </c>
+      <c r="C11" t="str">
+        <v>1:00</v>
+      </c>
+      <c r="D11" t="str">
+        <v>2:30</v>
+      </c>
+      <c r="E11" t="str">
+        <v xml:space="preserve">nap </v>
+      </c>
+      <c r="F11" t="str">
+        <v xml:space="preserve">weekly </v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v xml:space="preserve">dark dark blue </v>
+      </c>
+      <c r="B12" t="str">
+        <v>Thur</v>
+      </c>
+      <c r="C12" t="str">
+        <v>1:00</v>
+      </c>
+      <c r="D12" t="str">
+        <v>2:30</v>
+      </c>
+      <c r="E12" t="str">
+        <v xml:space="preserve">nap </v>
+      </c>
+      <c r="F12" t="str">
+        <v xml:space="preserve">weekly </v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v xml:space="preserve">dark dark blue </v>
+      </c>
+      <c r="B13" t="str">
+        <v>Fri</v>
+      </c>
+      <c r="C13" t="str">
+        <v>1:00</v>
+      </c>
+      <c r="D13" t="str">
+        <v>2:30</v>
+      </c>
+      <c r="E13" t="str">
+        <v xml:space="preserve">nap </v>
+      </c>
+      <c r="F13" t="str">
+        <v xml:space="preserve">weekly </v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>dark orange</v>
+      </c>
+      <c r="C14" t="str">
+        <v>1:00</v>
+      </c>
+      <c r="D14" t="str">
+        <v>2:00</v>
+      </c>
+      <c r="E14" t="str">
+        <v xml:space="preserve">nap </v>
+      </c>
+      <c r="F14" t="str">
+        <v xml:space="preserve">weekly </v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v xml:space="preserve">dark purple </v>
+      </c>
+      <c r="B15" t="str">
+        <v>Mon</v>
+      </c>
+      <c r="C15" t="str">
+        <v>3:00</v>
+      </c>
+      <c r="E15" t="str">
+        <v xml:space="preserve">leaves early </v>
+      </c>
+      <c r="F15" t="str">
+        <v>once</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v xml:space="preserve">light orange </v>
+      </c>
+      <c r="B16" t="str">
+        <v xml:space="preserve">Tue </v>
+      </c>
+      <c r="D16" t="str">
+        <v>10:15</v>
+      </c>
+      <c r="E16" t="str">
+        <v xml:space="preserve">late arrival </v>
+      </c>
+      <c r="F16" t="str">
+        <v xml:space="preserve">weekly </v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v xml:space="preserve">light orange </v>
+      </c>
+      <c r="B17" t="str">
+        <v>Thur</v>
+      </c>
+      <c r="D17" t="str">
+        <v>10:15</v>
+      </c>
+      <c r="E17" t="str">
+        <v xml:space="preserve">late arrival </v>
+      </c>
+      <c r="F17" t="str">
+        <v xml:space="preserve">weekly </v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F17"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Role</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v xml:space="preserve">Mario </v>
+      </c>
+      <c r="B2" t="str">
+        <v>Tech</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Luigi</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Tech</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v xml:space="preserve">Peach </v>
+      </c>
+      <c r="B4" t="str">
+        <v>Tech</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v xml:space="preserve">Daisy </v>
+      </c>
+      <c r="B5" t="str">
+        <v>Tech</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v xml:space="preserve">Toad </v>
+      </c>
+      <c r="B6" t="str">
+        <v>Tech</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v xml:space="preserve">Bowser </v>
+      </c>
+      <c r="B7" t="str">
+        <v>Tech</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>SBT _1</v>
+      </c>
+      <c r="B8" t="str">
+        <v>SBT</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Frodo</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Tech</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Sam</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Tech</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Legolas</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Tech</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Gimli</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Tech</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>Aragorn</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Tech</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v xml:space="preserve">Gandalf </v>
+      </c>
+      <c r="B14" t="str">
+        <v>Tech</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Thor</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Tech</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Iron Man</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Tech</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v xml:space="preserve">Black Widow </v>
+      </c>
+      <c r="B17" t="str">
+        <v>Tech</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v xml:space="preserve">Hulk </v>
+      </c>
+      <c r="B18" t="str">
+        <v>Tech</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>Spiderman</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Tech</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>SBT_2</v>
+      </c>
+      <c r="B20" t="str">
+        <v>SBT</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v xml:space="preserve">Arrow </v>
+      </c>
+      <c r="B21" t="str">
+        <v>Tech</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v xml:space="preserve">Batman </v>
+      </c>
+      <c r="B22" t="str">
+        <v>Tech</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>Superman</v>
+      </c>
+      <c r="B23" t="str">
+        <v>Tech</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v xml:space="preserve">Flash </v>
+      </c>
+      <c r="B24" t="str">
+        <v>Tech</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>TS_1</v>
+      </c>
+      <c r="B25" t="str">
+        <v>TS</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>TS_2</v>
+      </c>
+      <c r="B26" t="str">
+        <v>TS</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>TS_3</v>
+      </c>
+      <c r="B27" t="str">
+        <v>TS</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>BS</v>
+      </c>
+      <c r="B28" t="str">
+        <v>BS</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v xml:space="preserve">OM </v>
+      </c>
+      <c r="B29" t="str">
+        <v>OM</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>SBA1</v>
+      </c>
+      <c r="B30" t="str">
+        <v>SBA</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>SBA2</v>
+      </c>
+      <c r="B31" t="str">
+        <v>SBA</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>SBA3</v>
+      </c>
+      <c r="B32" t="str">
+        <v>SBA</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:B32"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>description</v>
+      </c>
+      <c r="C1" t="str">
+        <v xml:space="preserve">importance </v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>dyad</v>
+      </c>
+      <c r="B2" t="str">
+        <v>two kids one tech. limited list of permitted tech-child-child groups</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>trainings</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v xml:space="preserve">dyad trainings </v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>sbt, ts</v>
+      </c>
+      <c r="B5" t="str">
+        <v>can work with any kid</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>short trains</v>
+      </c>
+      <c r="B6" t="str">
+        <v xml:space="preserve">can only work with client for 2hrs </v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v xml:space="preserve">cancelling kids </v>
+      </c>
+      <c r="C7" t="str">
+        <v>low</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v xml:space="preserve">training schedule -new tech </v>
+      </c>
+      <c r="B8" t="str">
+        <v>technician can't be alone with a child, must be with ts, bs, sba.</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v xml:space="preserve">new client </v>
+      </c>
+      <c r="B9" t="str">
+        <v xml:space="preserve">goes to training specialist, bs, or sba first week </v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>training  schedule- current tech</v>
+      </c>
+      <c r="B10" t="str">
+        <v xml:space="preserve">typically training is 3-4 days does not include onboarding </v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v xml:space="preserve">client schedules </v>
+      </c>
+      <c r="B11" t="str">
+        <v xml:space="preserve">clients attending 1/2 day, coming in late, leaving early </v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>nap room coverage</v>
+      </c>
+      <c r="B12" t="str">
+        <v xml:space="preserve"> need 1 adult in the naproom, typically goes to TS/BS first before tech. Can have tech in there for 1 30 min block but not first choice </v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v xml:space="preserve">lunch break </v>
+      </c>
+      <c r="B13" t="str">
+        <v xml:space="preserve">earliest start 11:30, latest start 1:30 </v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v xml:space="preserve">session doc </v>
+      </c>
+      <c r="B14" t="str">
+        <v xml:space="preserve">last adul with kid when kid leaves needs to close them out. ideally right when kid leaves but should happen by end of hte day </v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:C14"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
@@ -877,4 +1743,419 @@
     <ignoredError numberStoredAsText="1" sqref="A1:E19"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AF19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="B1" t="str">
+        <v xml:space="preserve">Mario </v>
+      </c>
+      <c r="C1" t="str">
+        <v>Luigi</v>
+      </c>
+      <c r="D1" t="str">
+        <v xml:space="preserve">Peach </v>
+      </c>
+      <c r="E1" t="str">
+        <v xml:space="preserve">Daisy </v>
+      </c>
+      <c r="F1" t="str">
+        <v xml:space="preserve">Toad </v>
+      </c>
+      <c r="G1" t="str">
+        <v xml:space="preserve">Bowser </v>
+      </c>
+      <c r="H1" t="str">
+        <v>SBT _1</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Frodo</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Sam</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Legolas</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Gimli</v>
+      </c>
+      <c r="M1" t="str">
+        <v>Aragorn</v>
+      </c>
+      <c r="N1" t="str">
+        <v xml:space="preserve">Gandalf </v>
+      </c>
+      <c r="O1" t="str">
+        <v>Thor</v>
+      </c>
+      <c r="P1" t="str">
+        <v>Iron Man</v>
+      </c>
+      <c r="Q1" t="str">
+        <v xml:space="preserve">Black Widow </v>
+      </c>
+      <c r="R1" t="str">
+        <v xml:space="preserve">Hulk </v>
+      </c>
+      <c r="S1" t="str">
+        <v>Spiderman</v>
+      </c>
+      <c r="T1" t="str">
+        <v>SBT_2</v>
+      </c>
+      <c r="U1" t="str">
+        <v xml:space="preserve">Arrow </v>
+      </c>
+      <c r="V1" t="str">
+        <v xml:space="preserve">Batman </v>
+      </c>
+      <c r="W1" t="str">
+        <v>Superman</v>
+      </c>
+      <c r="X1" t="str">
+        <v xml:space="preserve">Flash </v>
+      </c>
+      <c r="Y1" t="str">
+        <v>TS_1</v>
+      </c>
+      <c r="Z1" t="str">
+        <v>TS_2</v>
+      </c>
+      <c r="AA1" t="str">
+        <v>TS_3</v>
+      </c>
+      <c r="AB1" t="str">
+        <v>BS</v>
+      </c>
+      <c r="AC1" t="str">
+        <v xml:space="preserve">OM </v>
+      </c>
+      <c r="AD1" t="str">
+        <v>SBA1</v>
+      </c>
+      <c r="AE1" t="str">
+        <v>SBA2</v>
+      </c>
+      <c r="AF1" t="str">
+        <v>SBA3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>8:30</v>
+      </c>
+      <c r="I2" t="str">
+        <v xml:space="preserve">pink </v>
+      </c>
+      <c r="T2" t="str">
+        <v xml:space="preserve">grey </v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>9:00</v>
+      </c>
+      <c r="M3" t="str">
+        <v xml:space="preserve">light blue </v>
+      </c>
+      <c r="X3" t="str">
+        <v>dark orange</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>9:30</v>
+      </c>
+      <c r="D4" t="str">
+        <v>light orange</v>
+      </c>
+      <c r="F4" t="str">
+        <v>red</v>
+      </c>
+      <c r="G4" t="str">
+        <v xml:space="preserve">pale yellow </v>
+      </c>
+      <c r="J4" t="str">
+        <v xml:space="preserve">dark green </v>
+      </c>
+      <c r="K4" t="str">
+        <v xml:space="preserve">light grey </v>
+      </c>
+      <c r="N4" t="str">
+        <v xml:space="preserve">yellow </v>
+      </c>
+      <c r="Y4" t="str">
+        <v xml:space="preserve">light grey </v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>10:00</v>
+      </c>
+      <c r="C5" t="str">
+        <v xml:space="preserve">tan </v>
+      </c>
+      <c r="E5" t="str">
+        <v xml:space="preserve">light purple </v>
+      </c>
+      <c r="H5" t="str">
+        <v xml:space="preserve">purple </v>
+      </c>
+      <c r="O5" t="str">
+        <v xml:space="preserve">teal </v>
+      </c>
+      <c r="P5" t="str">
+        <v xml:space="preserve">grey </v>
+      </c>
+      <c r="Q5" t="str">
+        <v xml:space="preserve">sky blue </v>
+      </c>
+      <c r="V5" t="str">
+        <v xml:space="preserve">dark dark blue </v>
+      </c>
+      <c r="W5" t="str">
+        <v xml:space="preserve">maroon </v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>10:30</v>
+      </c>
+      <c r="B6" t="str">
+        <v>green</v>
+      </c>
+      <c r="T6" t="str">
+        <v xml:space="preserve">dark pink </v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>11:00</v>
+      </c>
+      <c r="S7" t="str">
+        <v xml:space="preserve">dark purple </v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>11:30</v>
+      </c>
+      <c r="F8" t="str">
+        <v>light orange</v>
+      </c>
+      <c r="J8" t="str">
+        <v xml:space="preserve">pink </v>
+      </c>
+      <c r="X8" t="str">
+        <v xml:space="preserve">dark green/dark orange dyad </v>
+      </c>
+      <c r="Z8" t="str">
+        <v xml:space="preserve">dark blue </v>
+      </c>
+      <c r="AC8" t="str">
+        <v xml:space="preserve">pale yellow </v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>12:00</v>
+      </c>
+      <c r="E9" t="str">
+        <v>red</v>
+      </c>
+      <c r="G9" t="str">
+        <v xml:space="preserve">pale yellow </v>
+      </c>
+      <c r="M9" t="str">
+        <v xml:space="preserve">grey </v>
+      </c>
+      <c r="P9" t="str">
+        <v xml:space="preserve">light blue </v>
+      </c>
+      <c r="T9" t="str">
+        <v>yellow/dark pink dyad</v>
+      </c>
+      <c r="X9" t="str">
+        <v xml:space="preserve">dark orange </v>
+      </c>
+      <c r="AB9" t="str">
+        <v xml:space="preserve">light purple </v>
+      </c>
+      <c r="AC9" t="str">
+        <v>tan</v>
+      </c>
+      <c r="AD9" t="str">
+        <v>dark blue/maroon dyad</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>12:30</v>
+      </c>
+      <c r="D10" t="str">
+        <v xml:space="preserve">green </v>
+      </c>
+      <c r="I10" t="str">
+        <v xml:space="preserve">dark green </v>
+      </c>
+      <c r="N10" t="str">
+        <v>grey/skyblue</v>
+      </c>
+      <c r="Z10" t="str">
+        <v>tan</v>
+      </c>
+      <c r="AB10" t="str">
+        <v>yellow</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>13:00</v>
+      </c>
+      <c r="C11" t="str">
+        <v xml:space="preserve">light purple </v>
+      </c>
+      <c r="K11" t="str">
+        <v xml:space="preserve">pink </v>
+      </c>
+      <c r="N11" t="str">
+        <v xml:space="preserve">grey </v>
+      </c>
+      <c r="R11" t="str">
+        <v xml:space="preserve">dark purple </v>
+      </c>
+      <c r="S11" t="str">
+        <v xml:space="preserve">dark pink </v>
+      </c>
+      <c r="T11" t="str">
+        <v>sky blue</v>
+      </c>
+      <c r="W11" t="str">
+        <v xml:space="preserve">maroon </v>
+      </c>
+      <c r="AD11" t="str">
+        <v>teal</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>13:30</v>
+      </c>
+      <c r="B12" t="str">
+        <v xml:space="preserve">dark blue </v>
+      </c>
+      <c r="Y12" t="str">
+        <v xml:space="preserve">pink </v>
+      </c>
+      <c r="Z12" t="str">
+        <v>teal</v>
+      </c>
+      <c r="AB12" t="str">
+        <v>light orange</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>14:00</v>
+      </c>
+      <c r="C13" t="str">
+        <v xml:space="preserve">dark green </v>
+      </c>
+      <c r="H13" t="str">
+        <v>light orange</v>
+      </c>
+      <c r="J13" t="str">
+        <v xml:space="preserve">pink </v>
+      </c>
+      <c r="M13" t="str">
+        <v xml:space="preserve">light grey </v>
+      </c>
+      <c r="T13" t="str">
+        <v xml:space="preserve">dark purple </v>
+      </c>
+      <c r="X13" t="str">
+        <v xml:space="preserve">maroon </v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>14:30</v>
+      </c>
+      <c r="C14" t="str">
+        <v>2:45</v>
+      </c>
+      <c r="E14" t="str">
+        <v xml:space="preserve">light purple </v>
+      </c>
+      <c r="I14" t="str">
+        <v xml:space="preserve">light blue </v>
+      </c>
+      <c r="O14" t="str">
+        <v xml:space="preserve">purple </v>
+      </c>
+      <c r="Q14" t="str">
+        <v xml:space="preserve">yellow </v>
+      </c>
+      <c r="R14" t="str">
+        <v xml:space="preserve">dark pink </v>
+      </c>
+      <c r="S14" t="str">
+        <v>teal</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>15:00</v>
+      </c>
+      <c r="F15" t="str">
+        <v xml:space="preserve">pale yellow </v>
+      </c>
+      <c r="G15" t="str">
+        <v xml:space="preserve">dark blue </v>
+      </c>
+      <c r="V15" t="str">
+        <v xml:space="preserve">tan </v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>15:30</v>
+      </c>
+      <c r="B16" t="str">
+        <v xml:space="preserve">green </v>
+      </c>
+      <c r="P16" t="str">
+        <v xml:space="preserve">sky blue </v>
+      </c>
+      <c r="W16" t="str">
+        <v xml:space="preserve">dark orange </v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>16:00</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>16:30</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>17:00</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:AF19"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>